<commit_message>
Actualizaciones al modelo de calidad
Se realizan correcciones en la plantilla del modelo de calidad y se realiza presentación en power point para poder explicar con mayor claridad,  el porque de la elección de este modelo de calidad, el que es calidad y más aspectos importantes de este tema
</commit_message>
<xml_diff>
--- a/docs/trim04/04_Modelo_de_Calidad/PL02 - Lista de chequeo producto software.xlsx
+++ b/docs/trim04/04_Modelo_de_Calidad/PL02 - Lista de chequeo producto software.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\TaskMasterPro\docs\trim04\04_Modelo_de_Calidad\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7eb5a46966f243cc/Documentos/ANALISIS Y DESARROLLO DE SOFTWARE (2919581)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEEDCC63-945F-4A57-9FB8-C47A4B28BDFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{CDE57F57-BE07-4CE3-A00A-C64B1BFED427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B961976-9015-4EBD-B5DC-40913D223B3C}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="772" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1206,7 +1206,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1437,6 +1437,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1808,8 +1811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59A635BB-A94A-407B-BBB0-F2B3339CC475}">
   <dimension ref="A2:P81"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:D14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14"/>
@@ -2001,10 +2004,10 @@
       <c r="C23" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="D23" s="55" t="s">
+      <c r="D23" s="84" t="s">
         <v>82</v>
       </c>
-      <c r="E23" s="55"/>
+      <c r="E23" s="84"/>
       <c r="F23" s="30" t="s">
         <v>149</v>
       </c>
@@ -2300,8 +2303,9 @@
     <mergeCell ref="B34:F34"/>
     <mergeCell ref="B35:F35"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
+  <pageSetup scale="65" fitToWidth="0" fitToHeight="0" pageOrder="overThenDown" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -2310,8 +2314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EC27DB5-F54D-4E92-8170-7A53853F8C0C}">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:D14"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -3258,7 +3262,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3266,8 +3269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:D14"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -3907,7 +3910,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3915,8 +3917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D51D51-DE4C-4B5C-90F6-8EADB68EB458}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:D14"/>
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -4023,6 +4025,5 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ultimos ajustes de conexion de backend con frontend deñ CRUD de proyectos
</commit_message>
<xml_diff>
--- a/docs/trim04/04_Modelo_de_Calidad/PL02 - Lista de chequeo producto software.xlsx
+++ b/docs/trim04/04_Modelo_de_Calidad/PL02 - Lista de chequeo producto software.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7eb5a46966f243cc/Documentos/ANALISIS Y DESARROLLO DE SOFTWARE (2919581)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\TaskMasterPro\docs\trim04\04_Modelo_de_Calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{CDE57F57-BE07-4CE3-A00A-C64B1BFED427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6B961976-9015-4EBD-B5DC-40913D223B3C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30FB38D5-38AF-4139-A049-FB4B57785524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="772" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="772" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja de Control" sheetId="5" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="152">
   <si>
     <t>Funcionalidad</t>
   </si>
@@ -323,9 +323,6 @@
     <t>No Cumple</t>
   </si>
   <si>
-    <t>En el III trimestre estaba planificado realizarlo, por motivos de estructura front-end se sometio a ajustes y quedo planificada su realización para el IV trimestre</t>
-  </si>
-  <si>
     <t>El sistema debe permitir al Administrador Crear Rol</t>
   </si>
   <si>
@@ -500,6 +497,15 @@
   </si>
   <si>
     <t>04/03/2025</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>Avances RF</t>
+  </si>
+  <si>
+    <t>17/04/2025</t>
   </si>
 </sst>
 </file>
@@ -1353,35 +1359,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1412,34 +1411,41 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1811,8 +1817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59A635BB-A94A-407B-BBB0-F2B3339CC475}">
   <dimension ref="A2:P81"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27:E27"/>
+    <sheetView showGridLines="0" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30:E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14"/>
@@ -1834,91 +1840,91 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6">
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
     </row>
     <row r="3" spans="2:6" ht="30.5">
-      <c r="B3" s="79" t="s">
+      <c r="B3" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
     </row>
     <row r="4" spans="2:6" ht="30.5">
-      <c r="B4" s="79" t="s">
+      <c r="B4" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="79"/>
-      <c r="D4" s="79"/>
-      <c r="E4" s="79"/>
-      <c r="F4" s="79"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
     </row>
     <row r="5" spans="2:6" ht="14.5" thickBot="1">
-      <c r="B5" s="80"/>
-      <c r="C5" s="80"/>
-      <c r="D5" s="80"/>
-      <c r="E5" s="80"/>
-      <c r="F5" s="80"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
     </row>
     <row r="6" spans="2:6" ht="14.5" thickTop="1">
       <c r="F6" s="10"/>
     </row>
     <row r="8" spans="2:6" ht="30.5">
-      <c r="B8" s="81" t="s">
+      <c r="B8" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="81"/>
-      <c r="D8" s="81"/>
-      <c r="E8" s="81"/>
-      <c r="F8" s="81"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="58"/>
     </row>
     <row r="10" spans="2:6" ht="14.5" thickBot="1"/>
     <row r="11" spans="2:6" ht="18.5" thickTop="1">
       <c r="B11" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="75" t="s">
+      <c r="C11" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="76"/>
-      <c r="E11" s="76"/>
-      <c r="F11" s="77"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="54"/>
     </row>
     <row r="12" spans="2:6" ht="18">
       <c r="B12" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="63" t="s">
+      <c r="C12" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="D12" s="64"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="65"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="61"/>
+      <c r="F12" s="62"/>
     </row>
     <row r="13" spans="2:6" ht="18.5" thickBot="1">
       <c r="B13" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="63" t="s">
+      <c r="C13" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="64"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="65"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="62"/>
     </row>
     <row r="14" spans="2:6" ht="60.75" customHeight="1" thickTop="1">
       <c r="B14" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="63" t="s">
+      <c r="C14" s="60" t="s">
         <v>80</v>
       </c>
-      <c r="D14" s="67"/>
+      <c r="D14" s="64"/>
       <c r="E14" s="13" t="s">
         <v>20</v>
       </c>
@@ -1930,10 +1936,10 @@
       <c r="B15" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="68" t="s">
+      <c r="C15" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="69"/>
+      <c r="D15" s="66"/>
       <c r="E15" s="15" t="s">
         <v>23</v>
       </c>
@@ -1943,8 +1949,8 @@
       <c r="B16" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="70"/>
-      <c r="D16" s="71"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="68"/>
       <c r="E16" s="17" t="s">
         <v>25</v>
       </c>
@@ -1954,8 +1960,8 @@
     </row>
     <row r="17" spans="2:16" ht="16" thickTop="1">
       <c r="B17" s="19"/>
-      <c r="C17" s="72"/>
-      <c r="D17" s="72"/>
+      <c r="C17" s="69"/>
+      <c r="D17" s="69"/>
     </row>
     <row r="18" spans="2:16" ht="19.899999999999999" customHeight="1"/>
     <row r="19" spans="2:16" ht="19.899999999999999" customHeight="1">
@@ -1974,10 +1980,10 @@
       <c r="C21" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="73" t="s">
+      <c r="D21" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="73"/>
+      <c r="E21" s="70"/>
       <c r="F21" s="24" t="s">
         <v>31</v>
       </c>
@@ -1989,76 +1995,84 @@
       <c r="C22" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="74" t="s">
+      <c r="D22" s="71" t="s">
         <v>82</v>
       </c>
-      <c r="E22" s="74"/>
+      <c r="E22" s="71"/>
       <c r="F22" s="27" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="23" spans="2:16" ht="25.5" customHeight="1">
       <c r="B23" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="C23" s="29" t="s">
         <v>147</v>
       </c>
-      <c r="C23" s="29" t="s">
+      <c r="D23" s="72" t="s">
+        <v>82</v>
+      </c>
+      <c r="E23" s="72"/>
+      <c r="F23" s="30" t="s">
         <v>148</v>
       </c>
-      <c r="D23" s="84" t="s">
+    </row>
+    <row r="24" spans="2:16" ht="25.5" customHeight="1">
+      <c r="B24" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="D24" s="59" t="s">
         <v>82</v>
       </c>
-      <c r="E23" s="84"/>
-      <c r="F23" s="30" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="24" spans="2:16" ht="25.5" customHeight="1">
-      <c r="B24" s="28"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="55"/>
-      <c r="E24" s="55"/>
-      <c r="F24" s="30"/>
+      <c r="E24" s="59"/>
+      <c r="F24" s="30" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="25" spans="2:16" ht="25.5" customHeight="1">
       <c r="B25" s="28"/>
       <c r="C25" s="29"/>
-      <c r="D25" s="55"/>
-      <c r="E25" s="55"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
       <c r="F25" s="30"/>
     </row>
     <row r="26" spans="2:16" ht="25.5" customHeight="1">
       <c r="B26" s="28"/>
       <c r="C26" s="29"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="55"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="59"/>
       <c r="F26" s="30"/>
     </row>
     <row r="27" spans="2:16" ht="25.5" customHeight="1">
       <c r="B27" s="28"/>
       <c r="C27" s="29"/>
-      <c r="D27" s="55"/>
-      <c r="E27" s="55"/>
+      <c r="D27" s="59"/>
+      <c r="E27" s="59"/>
       <c r="F27" s="30"/>
     </row>
     <row r="28" spans="2:16" ht="25.5" customHeight="1">
       <c r="B28" s="28"/>
       <c r="C28" s="29"/>
-      <c r="D28" s="55"/>
-      <c r="E28" s="55"/>
+      <c r="D28" s="59"/>
+      <c r="E28" s="59"/>
       <c r="F28" s="30"/>
     </row>
     <row r="29" spans="2:16" ht="25.5" customHeight="1">
       <c r="B29" s="28"/>
       <c r="C29" s="29"/>
-      <c r="D29" s="55"/>
-      <c r="E29" s="55"/>
+      <c r="D29" s="59"/>
+      <c r="E29" s="59"/>
       <c r="F29" s="30"/>
     </row>
     <row r="30" spans="2:16" ht="25.5" customHeight="1" thickBot="1">
       <c r="B30" s="31"/>
       <c r="C30" s="32"/>
-      <c r="D30" s="56"/>
-      <c r="E30" s="56"/>
+      <c r="D30" s="76"/>
+      <c r="E30" s="76"/>
       <c r="F30" s="33"/>
     </row>
     <row r="31" spans="2:16" ht="19.899999999999999" customHeight="1" thickTop="1"/>
@@ -2069,52 +2083,52 @@
     </row>
     <row r="33" spans="1:13" ht="30" customHeight="1" thickBot="1"/>
     <row r="34" spans="1:13" ht="19.899999999999999" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B34" s="57" t="s">
+      <c r="B34" s="77" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="58"/>
-      <c r="D34" s="58"/>
-      <c r="E34" s="58"/>
-      <c r="F34" s="59"/>
+      <c r="C34" s="78"/>
+      <c r="D34" s="78"/>
+      <c r="E34" s="78"/>
+      <c r="F34" s="79"/>
     </row>
     <row r="35" spans="1:13" s="34" customFormat="1" ht="25.5" customHeight="1" thickTop="1">
-      <c r="B35" s="60" t="s">
+      <c r="B35" s="80" t="s">
         <v>82</v>
       </c>
-      <c r="C35" s="61"/>
-      <c r="D35" s="61"/>
-      <c r="E35" s="61"/>
-      <c r="F35" s="62"/>
+      <c r="C35" s="81"/>
+      <c r="D35" s="81"/>
+      <c r="E35" s="81"/>
+      <c r="F35" s="82"/>
     </row>
     <row r="36" spans="1:13" s="34" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B36" s="52" t="s">
+      <c r="B36" s="73" t="s">
         <v>83</v>
       </c>
-      <c r="C36" s="53"/>
-      <c r="D36" s="53"/>
-      <c r="E36" s="53"/>
-      <c r="F36" s="54"/>
+      <c r="C36" s="74"/>
+      <c r="D36" s="74"/>
+      <c r="E36" s="74"/>
+      <c r="F36" s="75"/>
       <c r="J36" s="34" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:13" s="34" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B37" s="52" t="s">
+      <c r="B37" s="73" t="s">
         <v>84</v>
       </c>
-      <c r="C37" s="53"/>
-      <c r="D37" s="53"/>
-      <c r="E37" s="53"/>
-      <c r="F37" s="54"/>
+      <c r="C37" s="74"/>
+      <c r="D37" s="74"/>
+      <c r="E37" s="74"/>
+      <c r="F37" s="75"/>
     </row>
     <row r="38" spans="1:13" s="34" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B38" s="52" t="s">
+      <c r="B38" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="C38" s="53"/>
-      <c r="D38" s="53"/>
-      <c r="E38" s="53"/>
-      <c r="F38" s="54"/>
+      <c r="C38" s="74"/>
+      <c r="D38" s="74"/>
+      <c r="E38" s="74"/>
+      <c r="F38" s="75"/>
     </row>
     <row r="39" spans="1:13" ht="19.899999999999999" customHeight="1">
       <c r="A39" s="34"/>
@@ -2275,12 +2289,15 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B35:F35"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="C12:F12"/>
     <mergeCell ref="C13:F13"/>
@@ -2293,19 +2310,16 @@
     <mergeCell ref="D23:E23"/>
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="D25:E25"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B8:F8"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
-  <pageSetup scale="65" fitToWidth="0" fitToHeight="0" pageOrder="overThenDown" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="3" scale="65" fitToWidth="0" fitToHeight="0" pageOrder="overThenDown" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -2314,8 +2328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EC27DB5-F54D-4E92-8170-7A53853F8C0C}">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -2373,10 +2387,11 @@
         <v>89</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="D4" s="50" t="s">
-        <v>91</v>
+        <v>87</v>
+      </c>
+      <c r="D4" s="6" t="str">
+        <f t="shared" ref="D4:D17" si="0">IF(C4="Cumple","Ninguna","")</f>
+        <v>Ninguna</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
@@ -2384,13 +2399,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>87</v>
       </c>
       <c r="D5" s="6" t="str">
-        <f t="shared" ref="D5:D17" si="0">IF(C5="Cumple","Ninguna","")</f>
+        <f t="shared" si="0"/>
         <v>Ninguna</v>
       </c>
     </row>
@@ -2399,7 +2414,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>87</v>
@@ -2414,7 +2429,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>87</v>
@@ -2429,7 +2444,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>87</v>
@@ -2444,7 +2459,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>87</v>
@@ -2459,7 +2474,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>87</v>
@@ -2474,7 +2489,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>87</v>
@@ -2489,7 +2504,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>87</v>
@@ -2504,7 +2519,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>87</v>
@@ -2519,7 +2534,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>87</v>
@@ -2534,7 +2549,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>87</v>
@@ -2549,7 +2564,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>87</v>
@@ -2564,7 +2579,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>87</v>
@@ -2579,7 +2594,7 @@
         <v>42</v>
       </c>
       <c r="B18" s="43" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C18" s="41"/>
       <c r="D18" s="42"/>
@@ -2603,14 +2618,14 @@
         <v>16</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D20" s="6" t="str">
         <f t="shared" ref="D20:D33" si="1">IF(C20="Cumple","Ninguna","")</f>
-        <v/>
+        <v>Ninguna</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
@@ -2618,7 +2633,7 @@
         <v>17</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>90</v>
@@ -2633,7 +2648,7 @@
         <v>18</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>90</v>
@@ -2648,14 +2663,14 @@
         <v>19</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D23" s="6" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Ninguna</v>
       </c>
     </row>
     <row r="24" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
@@ -2663,14 +2678,14 @@
         <v>20</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D24" s="6" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Ninguna</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
@@ -2678,14 +2693,14 @@
         <v>21</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D25" s="6" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Ninguna</v>
       </c>
     </row>
     <row r="26" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
@@ -2693,14 +2708,14 @@
         <v>22</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D26" s="6" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Ninguna</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
@@ -2708,7 +2723,7 @@
         <v>23</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>90</v>
@@ -2723,14 +2738,14 @@
         <v>24</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D28" s="6" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Ninguna</v>
       </c>
     </row>
     <row r="29" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
@@ -2738,14 +2753,14 @@
         <v>25</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D29" s="6" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Ninguna</v>
       </c>
     </row>
     <row r="30" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
@@ -2753,14 +2768,14 @@
         <v>26</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D30" s="6" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Ninguna</v>
       </c>
     </row>
     <row r="31" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
@@ -2768,7 +2783,7 @@
         <v>27</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>90</v>
@@ -2783,7 +2798,7 @@
         <v>28</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>90</v>
@@ -2798,7 +2813,7 @@
         <v>29</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>90</v>
@@ -2813,7 +2828,7 @@
         <v>42</v>
       </c>
       <c r="B34" s="43" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C34" s="41"/>
       <c r="D34" s="42"/>
@@ -2837,7 +2852,7 @@
         <v>31</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C36" s="5" t="s">
         <v>90</v>
@@ -2852,7 +2867,7 @@
         <v>32</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>90</v>
@@ -2867,7 +2882,7 @@
         <v>33</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>90</v>
@@ -2882,7 +2897,7 @@
         <v>34</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>90</v>
@@ -2897,7 +2912,7 @@
         <v>35</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>90</v>
@@ -2912,7 +2927,7 @@
         <v>36</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>90</v>
@@ -2927,7 +2942,7 @@
         <v>37</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>90</v>
@@ -2942,7 +2957,7 @@
         <v>38</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>90</v>
@@ -2957,7 +2972,7 @@
         <v>39</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>90</v>
@@ -2972,7 +2987,7 @@
         <v>42</v>
       </c>
       <c r="B45" s="43" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C45" s="41"/>
       <c r="D45" s="42"/>
@@ -2996,7 +3011,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>90</v>
@@ -3011,7 +3026,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>90</v>
@@ -3026,7 +3041,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>90</v>
@@ -3041,7 +3056,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>90</v>
@@ -3056,7 +3071,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="50" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>90</v>
@@ -3071,7 +3086,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>90</v>
@@ -3086,7 +3101,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="50" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>90</v>
@@ -3101,7 +3116,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>90</v>
@@ -3116,7 +3131,7 @@
         <v>42</v>
       </c>
       <c r="B55" s="43" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C55" s="41"/>
       <c r="D55" s="42"/>
@@ -3140,7 +3155,7 @@
         <v>46</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>90</v>
@@ -3155,7 +3170,7 @@
         <v>47</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>90</v>
@@ -3170,7 +3185,7 @@
         <v>48</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>90</v>
@@ -3185,7 +3200,7 @@
         <v>49</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>90</v>
@@ -3200,7 +3215,7 @@
         <v>50</v>
       </c>
       <c r="B61" s="50" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C61" s="5" t="s">
         <v>90</v>
@@ -3215,7 +3230,7 @@
         <v>51</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>90</v>
@@ -3230,7 +3245,7 @@
         <v>52</v>
       </c>
       <c r="B63" s="50" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C63" s="5" t="s">
         <v>90</v>
@@ -3245,7 +3260,7 @@
         <v>53</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C64" s="5" t="s">
         <v>90</v>
@@ -3261,7 +3276,9 @@
       <formula1>"Cumple, No Cumple"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
+  <pageSetup paperSize="3" scale="65" pageOrder="overThenDown" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3269,8 +3286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -3909,7 +3926,9 @@
       <formula1>"Cumple, No Cumple"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
+  <pageSetup paperSize="3" scale="65" pageOrder="overThenDown" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3918,7 +3937,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D30" sqref="D30:E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -3945,7 +3964,7 @@
       <c r="E1" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="82" t="s">
+      <c r="F1" s="83" t="s">
         <v>45</v>
       </c>
     </row>
@@ -3962,13 +3981,13 @@
       </c>
       <c r="D2" s="5">
         <f>COUNTIF('Requisitos Funcionales'!C2:C64,"Cumple")</f>
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="E2" s="48">
         <f>D2/C2%</f>
-        <v>25.925925925925924</v>
-      </c>
-      <c r="F2" s="83"/>
+        <v>42.592592592592588</v>
+      </c>
+      <c r="F2" s="84"/>
     </row>
     <row r="3" spans="1:6" s="4" customFormat="1">
       <c r="A3" s="47">
@@ -3989,7 +4008,7 @@
         <f t="shared" ref="E3:E4" si="0">D3/C3%</f>
         <v>82.35294117647058</v>
       </c>
-      <c r="F3" s="83"/>
+      <c r="F3" s="84"/>
     </row>
     <row r="4" spans="1:6" s="4" customFormat="1">
       <c r="C4" s="46">
@@ -3998,11 +4017,11 @@
       </c>
       <c r="D4" s="46">
         <f>SUM(D2:D3)</f>
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="E4" s="49">
         <f t="shared" si="0"/>
-        <v>47.727272727272727</v>
+        <v>57.954545454545453</v>
       </c>
       <c r="F4" s="5" t="str">
         <f>IF(E4&gt;=90,"APROBADO",IF(AND(E4&gt;=70,E4&lt;90),"CORREGIR","NO APROBADO"))</f>
@@ -4024,6 +4043,8 @@
       <formula>"NO APROBADO"</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
+  <pageSetup paperSize="3" scale="65" pageOrder="overThenDown" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se actualiza documento de calidad
</commit_message>
<xml_diff>
--- a/docs/trim04/04_Modelo_de_Calidad/PL02 - Lista de chequeo producto software.xlsx
+++ b/docs/trim04/04_Modelo_de_Calidad/PL02 - Lista de chequeo producto software.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\TaskMasterPro\docs\trim04\04_Modelo_de_Calidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA0A0BB-C062-4C1A-AF60-96A62FB2FC6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C04F310C-6E1A-4F88-B0CF-CAD1549E040C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="772" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="149">
   <si>
     <t>Funcionalidad</t>
   </si>
@@ -233,9 +233,6 @@
     <t>¿Se definió la estrategia de detección y corrección de errores a causa de las fallas?</t>
   </si>
   <si>
-    <t xml:space="preserve">¿La capacidad del sistema para tolerar errores está especificada en los requisitos? </t>
-  </si>
-  <si>
     <t>¿Se tiene prevista la capacidad de protección contra el acceso de datos e información no autorizados, ya sea accidental o de_x0002_liberadamente?</t>
   </si>
   <si>
@@ -245,9 +242,6 @@
     <t>¿Se tiene previsto demostrar la identidad de un sujeto o un recurso?</t>
   </si>
   <si>
-    <t>¿Se incluye la respuesta del sistema a los cambios en el entorno operativo, las interfaces, la precisión, el rendimiento, y otras capacidades adicionales predecibles?</t>
-  </si>
-  <si>
     <t>¿Se incluye la manera en que el sistema interactuará con otros software?</t>
   </si>
   <si>
@@ -267,9 +261,6 @@
   </si>
   <si>
     <t>¿Se ha especificado un panorama general respecto a la interfaz del sistema/software, como: colores, fuentes, logos?</t>
-  </si>
-  <si>
-    <t>¿Se han definido las interfaces externas, como por ejemplo usuarios o hardware?</t>
   </si>
   <si>
     <t>¿Se han definido las interfaces internas, como por ejemplo el software o el hardware?</t>
@@ -398,9 +389,6 @@
     <t>El sistema debe permitir al Administrador, Lider de poyecto y Miembro de proyecto Filtrar Proyecto</t>
   </si>
   <si>
-    <t xml:space="preserve">El sistema debe permitir al Administrador y Lider de proyecto Gestionar Permisos </t>
-  </si>
-  <si>
     <t>El sistema debe permitir al Administrador y Lider de proyecto Agregar Miembros de Proyecto</t>
   </si>
   <si>
@@ -463,9 +451,6 @@
     <t>El sistema debe permitir al Administrador, Lider de proyecto y Miembro de proyecto Adjuntar Archivos desde Servicios de Almacenamiento en la Nube</t>
   </si>
   <si>
-    <t>PERSONALIZACIÓJN</t>
-  </si>
-  <si>
     <t>El sistema deberá permitir al Administrador y Lider de proyecto Agregar Campos Personalizados a formularios de creacion de  proyectos o tareas</t>
   </si>
   <si>
@@ -506,6 +491,12 @@
   </si>
   <si>
     <t>17/04/2025</t>
+  </si>
+  <si>
+    <t>El sistema debe permitir al Administrador, Lider de proyecto, Miembro de proyecto y cliente/StakeHolder Modificar su Contraseña en la edición de su perfil</t>
+  </si>
+  <si>
+    <t>PERSONALIZACIÓN</t>
   </si>
 </sst>
 </file>
@@ -1359,35 +1350,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1421,34 +1405,41 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1820,7 +1811,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59A635BB-A94A-407B-BBB0-F2B3339CC475}">
   <dimension ref="A2:P81"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="C17" sqref="C17:D17"/>
     </sheetView>
   </sheetViews>
@@ -1843,106 +1834,106 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6">
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
     </row>
     <row r="3" spans="2:6" ht="30.5">
-      <c r="B3" s="80" t="s">
+      <c r="B3" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
     </row>
     <row r="4" spans="2:6" ht="30.5">
-      <c r="B4" s="80" t="s">
+      <c r="B4" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="80"/>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
-      <c r="F4" s="80"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
     </row>
     <row r="5" spans="2:6" ht="14.5" thickBot="1">
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
-      <c r="F5" s="81"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
     </row>
     <row r="6" spans="2:6" ht="14.5" thickTop="1">
       <c r="F6" s="10"/>
     </row>
     <row r="8" spans="2:6" ht="30.5">
-      <c r="B8" s="82" t="s">
+      <c r="B8" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="82"/>
-      <c r="D8" s="82"/>
-      <c r="E8" s="82"/>
-      <c r="F8" s="82"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="58"/>
     </row>
     <row r="10" spans="2:6" ht="14.5" thickBot="1"/>
     <row r="11" spans="2:6" ht="18.5" thickTop="1">
       <c r="B11" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="76" t="s">
+      <c r="C11" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="77"/>
-      <c r="E11" s="77"/>
-      <c r="F11" s="78"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="54"/>
     </row>
     <row r="12" spans="2:6" ht="18">
       <c r="B12" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="63" t="s">
-        <v>79</v>
-      </c>
-      <c r="D12" s="64"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="65"/>
+      <c r="C12" s="60" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="61"/>
+      <c r="E12" s="61"/>
+      <c r="F12" s="62"/>
     </row>
     <row r="13" spans="2:6" ht="18.5" thickBot="1">
       <c r="B13" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="63" t="s">
+      <c r="C13" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="64"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="65"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="62"/>
     </row>
     <row r="14" spans="2:6" ht="60.75" customHeight="1" thickTop="1">
       <c r="B14" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="63" t="s">
-        <v>80</v>
-      </c>
-      <c r="D14" s="67"/>
+      <c r="C14" s="60" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" s="64"/>
       <c r="E14" s="13" t="s">
         <v>20</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="19.899999999999999" customHeight="1">
       <c r="B15" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="68" t="s">
+      <c r="C15" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="69"/>
+      <c r="D15" s="66"/>
       <c r="E15" s="15" t="s">
         <v>23</v>
       </c>
@@ -1952,8 +1943,8 @@
       <c r="B16" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="70"/>
-      <c r="D16" s="71"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="68"/>
       <c r="E16" s="17" t="s">
         <v>25</v>
       </c>
@@ -1963,8 +1954,8 @@
     </row>
     <row r="17" spans="2:16" ht="16" thickTop="1">
       <c r="B17" s="19"/>
-      <c r="C17" s="72"/>
-      <c r="D17" s="72"/>
+      <c r="C17" s="69"/>
+      <c r="D17" s="69"/>
     </row>
     <row r="18" spans="2:16" ht="19.899999999999999" customHeight="1"/>
     <row r="19" spans="2:16" ht="19.899999999999999" customHeight="1">
@@ -1983,10 +1974,10 @@
       <c r="C21" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="73" t="s">
+      <c r="D21" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="73"/>
+      <c r="E21" s="70"/>
       <c r="F21" s="24" t="s">
         <v>31</v>
       </c>
@@ -1998,84 +1989,84 @@
       <c r="C22" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="74" t="s">
-        <v>82</v>
-      </c>
-      <c r="E22" s="74"/>
+      <c r="D22" s="71" t="s">
+        <v>79</v>
+      </c>
+      <c r="E22" s="71"/>
       <c r="F22" s="27" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="2:16" ht="25.5" customHeight="1">
       <c r="B23" s="28" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>147</v>
-      </c>
-      <c r="D23" s="75" t="s">
-        <v>82</v>
-      </c>
-      <c r="E23" s="75"/>
+        <v>142</v>
+      </c>
+      <c r="D23" s="72" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" s="72"/>
       <c r="F23" s="30" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="24" spans="2:16" ht="25.5" customHeight="1">
       <c r="B24" s="28" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>150</v>
-      </c>
-      <c r="D24" s="85" t="s">
-        <v>82</v>
-      </c>
-      <c r="E24" s="85"/>
+        <v>145</v>
+      </c>
+      <c r="D24" s="73" t="s">
+        <v>79</v>
+      </c>
+      <c r="E24" s="73"/>
       <c r="F24" s="30" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" spans="2:16" ht="25.5" customHeight="1">
       <c r="B25" s="28"/>
       <c r="C25" s="29"/>
-      <c r="D25" s="55"/>
-      <c r="E25" s="55"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
       <c r="F25" s="30"/>
     </row>
     <row r="26" spans="2:16" ht="25.5" customHeight="1">
       <c r="B26" s="28"/>
       <c r="C26" s="29"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="55"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="59"/>
       <c r="F26" s="30"/>
     </row>
     <row r="27" spans="2:16" ht="25.5" customHeight="1">
       <c r="B27" s="28"/>
       <c r="C27" s="29"/>
-      <c r="D27" s="55"/>
-      <c r="E27" s="55"/>
+      <c r="D27" s="59"/>
+      <c r="E27" s="59"/>
       <c r="F27" s="30"/>
     </row>
     <row r="28" spans="2:16" ht="25.5" customHeight="1">
       <c r="B28" s="28"/>
       <c r="C28" s="29"/>
-      <c r="D28" s="55"/>
-      <c r="E28" s="55"/>
+      <c r="D28" s="59"/>
+      <c r="E28" s="59"/>
       <c r="F28" s="30"/>
     </row>
     <row r="29" spans="2:16" ht="25.5" customHeight="1">
       <c r="B29" s="28"/>
       <c r="C29" s="29"/>
-      <c r="D29" s="55"/>
-      <c r="E29" s="55"/>
+      <c r="D29" s="59"/>
+      <c r="E29" s="59"/>
       <c r="F29" s="30"/>
     </row>
     <row r="30" spans="2:16" ht="25.5" customHeight="1" thickBot="1">
       <c r="B30" s="31"/>
       <c r="C30" s="32"/>
-      <c r="D30" s="56"/>
-      <c r="E30" s="56"/>
+      <c r="D30" s="77"/>
+      <c r="E30" s="77"/>
       <c r="F30" s="33"/>
     </row>
     <row r="31" spans="2:16" ht="19.899999999999999" customHeight="1" thickTop="1"/>
@@ -2086,52 +2077,52 @@
     </row>
     <row r="33" spans="1:13" ht="30" customHeight="1" thickBot="1"/>
     <row r="34" spans="1:13" ht="19.899999999999999" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B34" s="57" t="s">
+      <c r="B34" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="58"/>
-      <c r="D34" s="58"/>
-      <c r="E34" s="58"/>
-      <c r="F34" s="59"/>
+      <c r="C34" s="79"/>
+      <c r="D34" s="79"/>
+      <c r="E34" s="79"/>
+      <c r="F34" s="80"/>
     </row>
     <row r="35" spans="1:13" s="34" customFormat="1" ht="25.5" customHeight="1" thickTop="1">
-      <c r="B35" s="60" t="s">
-        <v>82</v>
-      </c>
-      <c r="C35" s="61"/>
-      <c r="D35" s="61"/>
-      <c r="E35" s="61"/>
-      <c r="F35" s="62"/>
+      <c r="B35" s="81" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35" s="82"/>
+      <c r="D35" s="82"/>
+      <c r="E35" s="82"/>
+      <c r="F35" s="83"/>
     </row>
     <row r="36" spans="1:13" s="34" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B36" s="52" t="s">
-        <v>83</v>
-      </c>
-      <c r="C36" s="53"/>
-      <c r="D36" s="53"/>
-      <c r="E36" s="53"/>
-      <c r="F36" s="54"/>
+      <c r="B36" s="74" t="s">
+        <v>80</v>
+      </c>
+      <c r="C36" s="75"/>
+      <c r="D36" s="75"/>
+      <c r="E36" s="75"/>
+      <c r="F36" s="76"/>
       <c r="J36" s="34" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:13" s="34" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B37" s="52" t="s">
-        <v>84</v>
-      </c>
-      <c r="C37" s="53"/>
-      <c r="D37" s="53"/>
-      <c r="E37" s="53"/>
-      <c r="F37" s="54"/>
+      <c r="B37" s="74" t="s">
+        <v>81</v>
+      </c>
+      <c r="C37" s="75"/>
+      <c r="D37" s="75"/>
+      <c r="E37" s="75"/>
+      <c r="F37" s="76"/>
     </row>
     <row r="38" spans="1:13" s="34" customFormat="1" ht="25.5" customHeight="1">
-      <c r="B38" s="52" t="s">
-        <v>85</v>
-      </c>
-      <c r="C38" s="53"/>
-      <c r="D38" s="53"/>
-      <c r="E38" s="53"/>
-      <c r="F38" s="54"/>
+      <c r="B38" s="74" t="s">
+        <v>82</v>
+      </c>
+      <c r="C38" s="75"/>
+      <c r="D38" s="75"/>
+      <c r="E38" s="75"/>
+      <c r="F38" s="76"/>
     </row>
     <row r="39" spans="1:13" ht="19.899999999999999" customHeight="1">
       <c r="A39" s="34"/>
@@ -2292,12 +2283,15 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B35:F35"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="C12:F12"/>
     <mergeCell ref="C13:F13"/>
@@ -2310,15 +2304,12 @@
     <mergeCell ref="D23:E23"/>
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="D25:E25"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B8:F8"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
@@ -2331,8 +2322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EC27DB5-F54D-4E92-8170-7A53853F8C0C}">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -2348,7 +2339,7 @@
         <v>42</v>
       </c>
       <c r="B1" s="43" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C1" s="41"/>
       <c r="D1" s="42"/>
@@ -2372,10 +2363,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D3" s="6" t="str">
         <f>IF(C3="Cumple","Ninguna","")</f>
@@ -2387,13 +2378,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D4" s="6" t="str">
-        <f t="shared" ref="D4:D17" si="0">IF(C4="Cumple","Ninguna","")</f>
+        <f t="shared" ref="D4:D18" si="0">IF(C4="Cumple","Ninguna","")</f>
         <v>Ninguna</v>
       </c>
     </row>
@@ -2402,13 +2393,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>91</v>
+        <v>147</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D5" s="6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D5" si="1">IF(C5="Cumple","Ninguna","")</f>
         <v>Ninguna</v>
       </c>
     </row>
@@ -2417,10 +2408,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D6" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2432,10 +2423,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D7" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2447,10 +2438,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D8" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2462,10 +2453,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D9" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2477,10 +2468,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D10" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2492,10 +2483,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D11" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2507,10 +2498,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D12" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2522,10 +2513,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D13" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2537,10 +2528,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D14" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2552,10 +2543,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D15" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2567,10 +2558,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D16" s="6" t="str">
         <f t="shared" si="0"/>
@@ -2582,53 +2573,53 @@
         <v>15</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D17" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Ninguna</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
-      <c r="A18" s="44" t="s">
+    <row r="18" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
+      <c r="A18" s="8">
+        <v>16</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Ninguna</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
+      <c r="A19" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="43" t="s">
-        <v>104</v>
-      </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="42"/>
-    </row>
-    <row r="19" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A19" s="45" t="s">
+      <c r="B19" s="43" t="s">
+        <v>101</v>
+      </c>
+      <c r="C19" s="41"/>
+      <c r="D19" s="42"/>
+    </row>
+    <row r="20" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A20" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="39" t="s">
+      <c r="B20" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="39" t="s">
+      <c r="C20" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="39" t="s">
+      <c r="D20" s="39" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
-      <c r="A20" s="8">
-        <v>16</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D20" s="6" t="str">
-        <f t="shared" ref="D20:D33" si="1">IF(C20="Cumple","Ninguna","")</f>
-        <v>Ninguna</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
@@ -2636,13 +2627,13 @@
         <v>17</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D21" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="D21:D33" si="2">IF(C21="Cumple","Ninguna","")</f>
         <v>Ninguna</v>
       </c>
     </row>
@@ -2651,13 +2642,13 @@
         <v>18</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D22" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Ninguna</v>
       </c>
     </row>
@@ -2666,13 +2657,13 @@
         <v>19</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D23" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Ninguna</v>
       </c>
     </row>
@@ -2681,13 +2672,13 @@
         <v>20</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D24" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Ninguna</v>
       </c>
     </row>
@@ -2696,13 +2687,13 @@
         <v>21</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D25" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Ninguna</v>
       </c>
     </row>
@@ -2711,13 +2702,13 @@
         <v>22</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D26" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Ninguna</v>
       </c>
     </row>
@@ -2726,14 +2717,14 @@
         <v>23</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D27" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <f t="shared" si="2"/>
+        <v>Ninguna</v>
       </c>
     </row>
     <row r="28" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
@@ -2741,13 +2732,13 @@
         <v>24</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D28" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Ninguna</v>
       </c>
     </row>
@@ -2756,13 +2747,13 @@
         <v>25</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D29" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Ninguna</v>
       </c>
     </row>
@@ -2771,13 +2762,13 @@
         <v>26</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D30" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Ninguna</v>
       </c>
     </row>
@@ -2786,14 +2777,14 @@
         <v>27</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D31" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <f t="shared" si="2"/>
+        <v>Ninguna</v>
       </c>
     </row>
     <row r="32" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
@@ -2801,14 +2792,14 @@
         <v>28</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D32" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <f t="shared" si="2"/>
+        <v>Ninguna</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
@@ -2816,14 +2807,14 @@
         <v>29</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D33" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <f t="shared" si="2"/>
+        <v>Ninguna</v>
       </c>
     </row>
     <row r="34" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
@@ -2831,7 +2822,7 @@
         <v>42</v>
       </c>
       <c r="B34" s="43" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C34" s="41"/>
       <c r="D34" s="42"/>
@@ -2852,136 +2843,136 @@
     </row>
     <row r="36" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A36" s="8">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D36" s="6" t="str">
-        <f t="shared" ref="D36:D44" si="2">IF(C36="Cumple","Ninguna","")</f>
+        <f t="shared" ref="D36:D44" si="3">IF(C36="Cumple","Ninguna","")</f>
         <v/>
       </c>
     </row>
     <row r="37" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A37" s="8">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D37" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="38" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A38" s="8">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D38" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="39" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A39" s="8">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D39" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="40" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A40" s="8">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D40" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="41" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A41" s="8">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D41" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="42" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A42" s="8">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D42" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="43" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A43" s="8">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D43" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="44" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A44" s="8">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D44" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -2990,7 +2981,7 @@
         <v>42</v>
       </c>
       <c r="B45" s="43" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C45" s="41"/>
       <c r="D45" s="42"/>
@@ -3011,121 +3002,121 @@
     </row>
     <row r="47" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A47" s="8">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D47" s="6" t="str">
-        <f t="shared" ref="D47:D54" si="3">IF(C47="Cumple","Ninguna","")</f>
+        <f t="shared" ref="D47:D54" si="4">IF(C47="Cumple","Ninguna","")</f>
         <v/>
       </c>
     </row>
     <row r="48" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A48" s="8">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D48" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="49" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A49" s="8">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D49" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="50" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A50" s="8">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D50" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="51" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A51" s="8">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B51" s="50" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D51" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="52" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A52" s="8">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D52" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="53" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A53" s="8">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B53" s="50" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D53" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="54" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A54" s="8">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D54" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -3134,7 +3125,7 @@
         <v>42</v>
       </c>
       <c r="B55" s="43" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="C55" s="41"/>
       <c r="D55" s="42"/>
@@ -3155,127 +3146,127 @@
     </row>
     <row r="57" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A57" s="8">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D57" s="6" t="str">
-        <f t="shared" ref="D57:D64" si="4">IF(C57="Cumple","Ninguna","")</f>
+        <f t="shared" ref="D57:D64" si="5">IF(C57="Cumple","Ninguna","")</f>
         <v/>
       </c>
     </row>
     <row r="58" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A58" s="8">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D58" s="6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="59" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A59" s="8">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D59" s="6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="60" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A60" s="8">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D60" s="6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="61" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A61" s="8">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B61" s="50" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D61" s="6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="62" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A62" s="8">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D62" s="6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="63" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A63" s="8">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B63" s="50" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D63" s="6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="64" spans="1:4" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A64" s="8">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D64" s="6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C17 C20:C33 C57:C64 C36:C44 C47:C54" xr:uid="{F381E73E-C892-4E35-A1B1-7DCF65F35B27}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C21:C33 C57:C64 C36:C44 C47:C54 C3:C18" xr:uid="{F381E73E-C892-4E35-A1B1-7DCF65F35B27}">
       <formula1>"Cumple, No Cumple"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3287,10 +3278,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -3323,7 +3314,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D2" s="6" t="str">
         <f>IF(C2="Cumple","Ninguna","")</f>
@@ -3332,28 +3323,28 @@
     </row>
     <row r="3" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
       <c r="A3" s="8">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B3" s="50" t="s">
         <v>46</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D3" s="6" t="str">
-        <f t="shared" ref="D3:D42" si="0">IF(C3="Cumple","Ninguna","")</f>
+        <f t="shared" ref="D3:D39" si="0">IF(C3="Cumple","Ninguna","")</f>
         <v>Ninguna</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
       <c r="A4" s="8">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B4" s="50" t="s">
         <v>47</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D4" s="6" t="str">
         <f t="shared" si="0"/>
@@ -3362,13 +3353,13 @@
     </row>
     <row r="5" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
       <c r="A5" s="8">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B5" s="50" t="s">
         <v>48</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D5" s="6" t="str">
         <f t="shared" si="0"/>
@@ -3391,13 +3382,13 @@
     </row>
     <row r="7" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
       <c r="A7" s="8">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7" s="50" t="s">
         <v>49</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D7" s="6" t="str">
         <f t="shared" si="0"/>
@@ -3406,13 +3397,13 @@
     </row>
     <row r="8" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
       <c r="A8" s="8">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B8" s="50" t="s">
         <v>50</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D8" s="6" t="str">
         <f t="shared" si="0"/>
@@ -3421,28 +3412,28 @@
     </row>
     <row r="9" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
       <c r="A9" s="8">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B9" s="50" t="s">
         <v>51</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D9" s="6" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Ninguna</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
       <c r="A10" s="8">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B10" s="50" t="s">
         <v>52</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D10" s="6" t="str">
         <f t="shared" si="0"/>
@@ -3465,13 +3456,13 @@
     </row>
     <row r="12" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
       <c r="A12" s="8">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B12" s="50" t="s">
         <v>53</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D12" s="6" t="str">
         <f t="shared" si="0"/>
@@ -3480,13 +3471,13 @@
     </row>
     <row r="13" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
       <c r="A13" s="8">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B13" s="50" t="s">
         <v>54</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D13" s="6" t="str">
         <f t="shared" si="0"/>
@@ -3495,13 +3486,13 @@
     </row>
     <row r="14" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
       <c r="A14" s="8">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B14" s="50" t="s">
         <v>55</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D14" s="6" t="str">
         <f t="shared" si="0"/>
@@ -3510,13 +3501,13 @@
     </row>
     <row r="15" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
       <c r="A15" s="8">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B15" s="50" t="s">
         <v>56</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D15" s="6" t="str">
         <f t="shared" si="0"/>
@@ -3525,13 +3516,13 @@
     </row>
     <row r="16" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
       <c r="A16" s="8">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B16" s="50" t="s">
         <v>57</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D16" s="6" t="str">
         <f t="shared" si="0"/>
@@ -3540,13 +3531,13 @@
     </row>
     <row r="17" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
       <c r="A17" s="8">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B17" s="50" t="s">
         <v>58</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D17" s="6" t="str">
         <f t="shared" si="0"/>
@@ -3569,13 +3560,13 @@
     </row>
     <row r="19" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
       <c r="A19" s="8">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B19" s="50" t="s">
         <v>59</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D19" s="6" t="str">
         <f t="shared" si="0"/>
@@ -3584,13 +3575,13 @@
     </row>
     <row r="20" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
       <c r="A20" s="8">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B20" s="50" t="s">
         <v>60</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D20" s="6" t="str">
         <f t="shared" si="0"/>
@@ -3599,57 +3590,57 @@
     </row>
     <row r="21" spans="1:4" s="4" customFormat="1" ht="30" customHeight="1">
       <c r="A21" s="8">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B21" s="50" t="s">
         <v>61</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D21" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="30" customHeight="1">
-      <c r="A22" s="8">
-        <v>28</v>
-      </c>
-      <c r="B22" s="50" t="s">
+    <row r="22" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A22" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="30" customHeight="1">
+      <c r="A23" s="8">
+        <v>19</v>
+      </c>
+      <c r="B23" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="D22" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A23" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="B23" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="39" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" s="39" t="s">
-        <v>5</v>
+      <c r="C23" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Ninguna</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="30" customHeight="1">
       <c r="A24" s="8">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B24" s="50" t="s">
         <v>63</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D24" s="6" t="str">
         <f t="shared" si="0"/>
@@ -3658,57 +3649,57 @@
     </row>
     <row r="25" spans="1:4" ht="30" customHeight="1">
       <c r="A25" s="8">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B25" s="50" t="s">
         <v>64</v>
       </c>
       <c r="C25" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Ninguna</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A26" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="30" customHeight="1">
+      <c r="A27" s="8">
+        <v>23</v>
+      </c>
+      <c r="B27" s="50" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="D25" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>Ninguna</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="30" customHeight="1">
-      <c r="A26" s="8">
-        <v>32</v>
-      </c>
-      <c r="B26" s="50" t="s">
-        <v>65</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D26" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>Ninguna</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A27" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="B27" s="39" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" s="39" t="s">
-        <v>4</v>
-      </c>
-      <c r="D27" s="39" t="s">
-        <v>5</v>
+      <c r="D27" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
     </row>
     <row r="28" spans="1:4" ht="30" customHeight="1">
       <c r="A28" s="8">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B28" s="50" t="s">
         <v>66</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D28" s="6" t="str">
         <f t="shared" si="0"/>
@@ -3717,87 +3708,87 @@
     </row>
     <row r="29" spans="1:4" ht="30" customHeight="1">
       <c r="A29" s="8">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B29" s="50" t="s">
         <v>67</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D29" s="6" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Ninguna</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="30" customHeight="1">
       <c r="A30" s="8">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B30" s="50" t="s">
         <v>68</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D30" s="6" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="30" customHeight="1">
-      <c r="A31" s="8">
-        <v>38</v>
-      </c>
-      <c r="B31" s="50" t="s">
-        <v>69</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D31" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>Ninguna</v>
+        <v>Ninguna</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A31" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="39" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="30" customHeight="1">
       <c r="A32" s="8">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="B32" s="50" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D32" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Ninguna</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="30" customHeight="1">
+      <c r="A33" s="8">
+        <v>28</v>
+      </c>
+      <c r="B33" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="C32" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D32" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>Ninguna</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A33" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="B33" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="39" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" s="39" t="s">
-        <v>5</v>
+      <c r="C33" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D33" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Ninguna</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="30" customHeight="1">
       <c r="A34" s="8">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B34" s="50" t="s">
         <v>71</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D34" s="6" t="str">
         <f t="shared" si="0"/>
@@ -3806,43 +3797,42 @@
     </row>
     <row r="35" spans="1:4" ht="30" customHeight="1">
       <c r="A35" s="8">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B35" s="50" t="s">
         <v>72</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D35" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Ninguna</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="30" customHeight="1">
-      <c r="A36" s="8">
-        <v>46</v>
-      </c>
-      <c r="B36" s="50" t="s">
-        <v>73</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D36" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>Ninguna</v>
+    <row r="36" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
+      <c r="A36" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" s="39" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="30" customHeight="1">
       <c r="A37" s="8">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="B37" s="50" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D37" s="6" t="str">
         <f t="shared" si="0"/>
@@ -3851,81 +3841,37 @@
     </row>
     <row r="38" spans="1:4" ht="30" customHeight="1">
       <c r="A38" s="8">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="B38" s="50" t="s">
+        <v>74</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D38" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Ninguna</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="30" customHeight="1">
+      <c r="A39" s="8">
+        <v>34</v>
+      </c>
+      <c r="B39" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="C38" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D38" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>Ninguna</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" s="3" customFormat="1" ht="30" customHeight="1">
-      <c r="A39" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="B39" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="C39" s="39" t="s">
-        <v>4</v>
-      </c>
-      <c r="D39" s="39" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="30" customHeight="1">
-      <c r="A40" s="8">
-        <v>53</v>
-      </c>
-      <c r="B40" s="50" t="s">
-        <v>76</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D40" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>Ninguna</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="30" customHeight="1">
-      <c r="A41" s="8">
-        <v>54</v>
-      </c>
-      <c r="B41" s="50" t="s">
-        <v>77</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D41" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>Ninguna</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="30" customHeight="1">
-      <c r="A42" s="8">
-        <v>57</v>
-      </c>
-      <c r="B42" s="50" t="s">
-        <v>78</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D42" s="6" t="str">
+      <c r="C39" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D39" s="6" t="str">
         <f t="shared" si="0"/>
         <v>Ninguna</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C24:C26 C12:C17 C40:C42 C34:C38 C28:C32 C19:C22 C7:C10 C2:C5" xr:uid="{28946FFD-2DE3-4AFF-8B02-311FA9F788A5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C23:C25 C12:C17 C37:C39 C19:C21 C7:C10 C2:C5 C27:C30 C32:C35" xr:uid="{28946FFD-2DE3-4AFF-8B02-311FA9F788A5}">
       <formula1>"Cumple, No Cumple"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3939,8 +3885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D51D51-DE4C-4B5C-90F6-8EADB68EB458}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30:E30"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -3967,7 +3913,7 @@
       <c r="E1" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="83" t="s">
+      <c r="F1" s="84" t="s">
         <v>45</v>
       </c>
     </row>
@@ -3984,13 +3930,13 @@
       </c>
       <c r="D2" s="5">
         <f>COUNTIF('Requisitos Funcionales'!C2:C64,"Cumple")</f>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E2" s="48">
         <f>D2/C2%</f>
-        <v>46.296296296296291</v>
-      </c>
-      <c r="F2" s="84"/>
+        <v>53.703703703703702</v>
+      </c>
+      <c r="F2" s="85"/>
     </row>
     <row r="3" spans="1:6" s="4" customFormat="1">
       <c r="A3" s="47">
@@ -4001,7 +3947,7 @@
       </c>
       <c r="C3" s="5">
         <f>COUNT('Requisitos No Funcionales'!A:A)</f>
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D3" s="5">
         <f>COUNTIF('Requisitos No Funcionales'!C:C,"Cumple")</f>
@@ -4009,22 +3955,22 @@
       </c>
       <c r="E3" s="48">
         <f t="shared" ref="E3:E4" si="0">D3/C3%</f>
-        <v>82.35294117647058</v>
-      </c>
-      <c r="F3" s="84"/>
+        <v>90.322580645161295</v>
+      </c>
+      <c r="F3" s="85"/>
     </row>
     <row r="4" spans="1:6" s="4" customFormat="1">
       <c r="C4" s="46">
         <f>SUM(C2:C3)</f>
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D4" s="46">
         <f>SUM(D2:D3)</f>
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E4" s="49">
         <f t="shared" si="0"/>
-        <v>60.227272727272727</v>
+        <v>67.058823529411768</v>
       </c>
       <c r="F4" s="5" t="str">
         <f>IF(E4&gt;=90,"APROBADO",IF(AND(E4&gt;=70,E4&lt;90),"CORREGIR","NO APROBADO"))</f>

</xml_diff>